<commit_message>
prepare for new R version
</commit_message>
<xml_diff>
--- a/inst/extdata/examples/xlsx/box-simple.xlsx
+++ b/inst/extdata/examples/xlsx/box-simple.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t xml:space="preserve">tab</t>
   </si>
@@ -48,7 +48,7 @@
     <t xml:space="preserve">y_title</t>
   </si>
   <si>
-    <t xml:space="preserve">toename in de kans om geraakt te worden t.o.v. het gemiddelde</t>
+    <t xml:space="preserve">toename in de kans om geraakt te worden t.o.v. het gemiddelde (%)</t>
   </si>
   <si>
     <t xml:space="preserve">turn</t>
@@ -76,6 +76,12 @@
   </si>
   <si>
     <t xml:space="preserve">rose</t>
+  </si>
+  <si>
+    <t xml:space="preserve">box_median_lab_suffix</t>
+  </si>
+  <si>
+    <t xml:space="preserve">\s%</t>
   </si>
   <si>
     <t xml:space="preserve">hline_dash</t>
@@ -557,19 +563,27 @@
         <v>23</v>
       </c>
       <c r="B13" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B14" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="1"/>
+      <c r="A15" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -587,31 +601,31 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="H1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="I1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2">

</xml_diff>